<commit_message>
Add cases for UCED
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_uced.xlsx
+++ b/ams/cases/ieee14/ieee14_uced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F975BC3-D287-BC4C-8864-8FF8FB33FA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AFC3DD-B4A6-DF49-B870-26402AAE9341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -25,13 +25,18 @@
     <sheet name="Region" sheetId="10" r:id="rId10"/>
     <sheet name="EDTSlot" sheetId="13" r:id="rId11"/>
     <sheet name="UCTSlot" sheetId="14" r:id="rId12"/>
+    <sheet name="SFR" sheetId="16" r:id="rId13"/>
+    <sheet name="SFRCost" sheetId="17" r:id="rId14"/>
+    <sheet name="SR" sheetId="18" r:id="rId15"/>
+    <sheet name="NSR" sheetId="19" r:id="rId16"/>
+    <sheet name="RTEDCFG" sheetId="15" r:id="rId17"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="294">
   <si>
     <t>uid</t>
   </si>
@@ -795,32 +800,28 @@
     <t>R30</t>
   </si>
   <si>
-    <t>for UC, ED</t>
+    <t>1, 1</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>1, 1</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>1.005, 1.005</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>1.01, 1.01</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>1.015, 1.015</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>1.02, 1.02</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>1.025, 1.025</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>td1</t>
@@ -872,18 +873,76 @@
   </si>
   <si>
     <t>sd</t>
+  </si>
+  <si>
+    <t>RTEDCFG1</t>
+  </si>
+  <si>
+    <t>du</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>cru</t>
+  </si>
+  <si>
+    <t>crd</t>
+  </si>
+  <si>
+    <t>RCOST_1</t>
+  </si>
+  <si>
+    <t>RCOST_2</t>
+  </si>
+  <si>
+    <t>RCOST_3</t>
+  </si>
+  <si>
+    <t>RCOST_4</t>
+  </si>
+  <si>
+    <t>RCOST_5</t>
+  </si>
+  <si>
+    <t>SR1</t>
+  </si>
+  <si>
+    <t>SR2</t>
+  </si>
+  <si>
+    <t>demand</t>
+  </si>
+  <si>
+    <t>NSR1</t>
+  </si>
+  <si>
+    <t>NSR2</t>
+  </si>
+  <si>
+    <t>SFR1</t>
+  </si>
+  <si>
+    <t>SFR2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1011,39 +1070,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1386,7 +1449,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1419,14 +1482,12 @@
       <c r="C2" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>254</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1484,7 +1545,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -1508,10 +1569,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1519,10 +1580,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D2" s="1">
         <v>60</v>
@@ -1533,10 +1594,10 @@
         <v>15</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D3" s="1">
         <v>60</v>
@@ -1547,10 +1608,10 @@
         <v>22</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="1">
         <v>60</v>
@@ -1561,10 +1622,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D5" s="1">
         <v>60</v>
@@ -1575,10 +1636,10 @@
         <v>30</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="1">
         <v>60</v>
@@ -1589,17 +1650,17 @@
         <v>34</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D7" s="1">
         <v>60</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1608,7 +1669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8DE934-58E4-5047-A795-90496D563932}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -1622,10 +1683,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1633,10 +1694,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D2" s="1">
         <v>60</v>
@@ -1647,10 +1708,10 @@
         <v>15</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D3" s="1">
         <v>60</v>
@@ -1661,10 +1722,10 @@
         <v>22</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="1">
         <v>60</v>
@@ -1675,10 +1736,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D5" s="1">
         <v>60</v>
@@ -1689,10 +1750,10 @@
         <v>30</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="1">
         <v>60</v>
@@ -1703,17 +1764,411 @@
         <v>34</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D7" s="1">
         <v>60</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DCD101-2671-4F48-972B-11EA0EF73763}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111A03E0-C10C-0D49-95E3-8985E6A9343A}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="15">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="15">
+        <v>0</v>
+      </c>
+      <c r="E2" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="15">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
+        <v>2</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="15">
+        <v>3</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
+        <v>4</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEFDE885-6D53-A84E-BDCB-CAB019D9A33F}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E2" s="7">
+        <v>5</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E3" s="7">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB7A23E-CBBD-454F-8F4F-269AE72EF5B7}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="E2" s="7">
+        <v>5</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="7">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C550E806-D813-8D4B-AC59-65815710FA39}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2389,7 +2844,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <ignoredErrors>
@@ -2402,8 +2857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+    <sheetView zoomScale="105" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2473,10 +2928,10 @@
         <v>253</v>
       </c>
       <c r="U1" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="V1" s="11" t="s">
         <v>261</v>
-      </c>
-      <c r="V1" s="11" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -2492,8 +2947,8 @@
       <c r="D2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" t="s">
-        <v>88</v>
+      <c r="E2" s="1">
+        <v>50</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -2557,8 +3012,8 @@
       <c r="D3" t="s">
         <v>97</v>
       </c>
-      <c r="E3" t="s">
-        <v>88</v>
+      <c r="E3" s="1">
+        <v>50</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -2622,8 +3077,8 @@
       <c r="D4" t="s">
         <v>100</v>
       </c>
-      <c r="E4" t="s">
-        <v>88</v>
+      <c r="E4" s="1">
+        <v>50</v>
       </c>
       <c r="F4" t="s">
         <v>40</v>
@@ -2687,8 +3142,8 @@
       <c r="D5" t="s">
         <v>104</v>
       </c>
-      <c r="E5" t="s">
-        <v>88</v>
+      <c r="E5" s="1">
+        <v>50</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -2740,10 +3195,10 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:S5" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:S1 A3:D5 A2:D2 F2:S2 F3:S5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2753,7 +3208,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2826,10 +3281,10 @@
         <v>253</v>
       </c>
       <c r="V1" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="W1" s="9" t="s">
         <v>261</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -2845,8 +3300,8 @@
       <c r="D2" t="s">
         <v>106</v>
       </c>
-      <c r="E2" t="s">
-        <v>88</v>
+      <c r="E2" s="1">
+        <v>200</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -2901,10 +3356,10 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:T2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:T1 A2:D2 F2:T2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3338,7 +3793,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:K12" numberStoredAsText="1"/>
@@ -4794,7 +5249,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:X21" numberStoredAsText="1"/>
@@ -4907,7 +5362,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:J3" numberStoredAsText="1"/>
@@ -4968,7 +5423,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:D3" numberStoredAsText="1"/>
@@ -5161,7 +5616,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:D1 G1:I1 A6:D6 A2:D2 G2:I2 A3:D3 G3:I3 A4:D4 G4:I4 A5:D5 G5:I5 G6:I6" numberStoredAsText="1"/>

</xml_diff>

<commit_message>
Move routine interval into routine config and remove model rtnconfig
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_uced.xlsx
+++ b/ams/cases/ieee14/ieee14_uced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AFC3DD-B4A6-DF49-B870-26402AAE9341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01DC3D7-7B52-B643-AAE3-B075143DBA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -29,14 +29,13 @@
     <sheet name="SFRCost" sheetId="17" r:id="rId14"/>
     <sheet name="SR" sheetId="18" r:id="rId15"/>
     <sheet name="NSR" sheetId="19" r:id="rId16"/>
-    <sheet name="RTEDCFG" sheetId="15" r:id="rId17"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="292">
   <si>
     <t>uid</t>
   </si>
@@ -801,27 +800,27 @@
   </si>
   <si>
     <t>1, 1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>1.005, 1.005</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>1.01, 1.01</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>1.015, 1.015</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>1.02, 1.02</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>1.025, 1.025</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>td1</t>
@@ -869,13 +868,7 @@
     <t>UCT6</t>
   </si>
   <si>
-    <t>dt</t>
-  </si>
-  <si>
     <t>sd</t>
-  </si>
-  <si>
-    <t>RTEDCFG1</t>
   </si>
   <si>
     <t>du</t>
@@ -930,19 +923,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1070,41 +1056,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1487,7 +1472,7 @@
       <c r="F2" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1545,7 +1530,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -1556,7 +1541,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1569,11 +1554,9 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="D1" s="12" t="s">
         <v>275</v>
       </c>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1585,9 +1568,7 @@
       <c r="C2" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="D2" s="1">
-        <v>60</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1599,9 +1580,7 @@
       <c r="C3" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="D3" s="1">
-        <v>60</v>
-      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1613,9 +1592,7 @@
       <c r="C4" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="D4" s="1">
-        <v>60</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1627,9 +1604,7 @@
       <c r="C5" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="D5" s="1">
-        <v>60</v>
-      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1641,9 +1616,7 @@
       <c r="C6" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="D6" s="1">
-        <v>60</v>
-      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1655,12 +1628,10 @@
       <c r="C7" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="D7" s="1">
-        <v>60</v>
-      </c>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1670,7 +1641,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1683,11 +1654,9 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="D1" s="12" t="s">
         <v>275</v>
       </c>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1699,9 +1668,7 @@
       <c r="C2" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="D2" s="1">
-        <v>60</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1713,9 +1680,7 @@
       <c r="C3" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="D3" s="1">
-        <v>60</v>
-      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1727,9 +1692,7 @@
       <c r="C4" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="D4" s="1">
-        <v>60</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1741,9 +1704,7 @@
       <c r="C5" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="D5" s="1">
-        <v>60</v>
-      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1755,9 +1716,7 @@
       <c r="C6" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="D6" s="1">
-        <v>60</v>
-      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1769,12 +1728,10 @@
       <c r="C7" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="D7" s="1">
-        <v>60</v>
-      </c>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1803,10 +1760,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>12</v>
@@ -1817,13 +1774,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E2" s="7">
         <v>0.05</v>
@@ -1840,13 +1797,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E3" s="7">
         <v>0.05</v>
@@ -1874,104 +1831,104 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="C2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15">
+      <c r="C3" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="14">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="15">
+      <c r="C4" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="14">
         <v>0</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E4" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
+        <v>3</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="15">
+      <c r="C5" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="14">
         <v>0</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E5" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15">
-        <v>2</v>
-      </c>
-      <c r="B4" s="15" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>4</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="15">
+      <c r="C6" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="14">
         <v>0</v>
       </c>
-      <c r="E4" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="15">
-        <v>3</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="15">
-        <v>0</v>
-      </c>
-      <c r="E5" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15">
-        <v>4</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>286</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="15">
-        <v>0</v>
-      </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>0</v>
       </c>
     </row>
@@ -2004,7 +1961,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>12</v>
@@ -2015,13 +1972,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E2" s="7">
         <v>5</v>
@@ -2035,13 +1992,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E3" s="7">
         <v>5</v>
@@ -2060,7 +2017,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2079,7 +2036,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>12</v>
@@ -2090,13 +2047,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E2" s="7">
         <v>5</v>
@@ -2110,62 +2067,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E3" s="7">
         <v>5</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C550E806-D813-8D4B-AC59-65815710FA39}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2844,7 +2758,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <ignoredErrors>
@@ -3195,7 +3109,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:S1 A3:D5 A2:D2 F2:S2 F3:S5" numberStoredAsText="1"/>
@@ -3356,7 +3270,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:T1 A2:D2 F2:T2" numberStoredAsText="1"/>
@@ -3793,7 +3707,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:K12" numberStoredAsText="1"/>
@@ -5249,7 +5163,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:X21" numberStoredAsText="1"/>
@@ -5362,7 +5276,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:J3" numberStoredAsText="1"/>
@@ -5423,7 +5337,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:D3" numberStoredAsText="1"/>
@@ -5616,7 +5530,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:D1 G1:I1 A6:D6 A2:D2 G2:I2 A3:D3 G3:I3 A4:D4 G4:I4 A5:D5 G5:I5 G6:I6" numberStoredAsText="1"/>

</xml_diff>

<commit_message>
Revise cases for UCED
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_uced.xlsx
+++ b/ams/cases/ieee14/ieee14_uced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01DC3D7-7B52-B643-AAE3-B075143DBA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE31FE1F-398B-1841-8090-1E6C624E3C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -25,17 +25,20 @@
     <sheet name="Region" sheetId="10" r:id="rId10"/>
     <sheet name="EDTSlot" sheetId="13" r:id="rId11"/>
     <sheet name="UCTSlot" sheetId="14" r:id="rId12"/>
-    <sheet name="SFR" sheetId="16" r:id="rId13"/>
-    <sheet name="SFRCost" sheetId="17" r:id="rId14"/>
-    <sheet name="SR" sheetId="18" r:id="rId15"/>
-    <sheet name="NSR" sheetId="19" r:id="rId16"/>
+    <sheet name="DCost" sheetId="20" r:id="rId13"/>
+    <sheet name="SFR" sheetId="16" r:id="rId14"/>
+    <sheet name="SFRCost" sheetId="17" r:id="rId15"/>
+    <sheet name="SR" sheetId="18" r:id="rId16"/>
+    <sheet name="SRCost" sheetId="21" r:id="rId17"/>
+    <sheet name="NSR" sheetId="19" r:id="rId18"/>
+    <sheet name="NSRCost" sheetId="22" r:id="rId19"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="376">
   <si>
     <t>uid</t>
   </si>
@@ -799,39 +802,12 @@
     <t>R30</t>
   </si>
   <si>
-    <t>1, 1</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.005, 1.005</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.01, 1.01</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.015, 1.015</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.02, 1.02</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.025, 1.025</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>td1</t>
   </si>
   <si>
     <t>td2</t>
   </si>
   <si>
-    <t>1.005, 1.005</t>
-  </si>
-  <si>
     <t>EDT1</t>
   </si>
   <si>
@@ -917,6 +893,279 @@
   </si>
   <si>
     <t>SFR2</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>StaticGen</t>
+  </si>
+  <si>
+    <t>Load factor in EDTSlot and UCTSlot sourced from ISO-NE day-ahead cleared hourly load on 2022 June 29</t>
+  </si>
+  <si>
+    <t>Minimum on/off time of generators were made up</t>
+  </si>
+  <si>
+    <t>0.641, 0</t>
+  </si>
+  <si>
+    <t>0.634, 0</t>
+  </si>
+  <si>
+    <t>0.623, 0</t>
+  </si>
+  <si>
+    <t>0.615, 0</t>
+  </si>
+  <si>
+    <t>0.62, 0</t>
+  </si>
+  <si>
+    <t>EDT7</t>
+  </si>
+  <si>
+    <t>0.665, 0</t>
+  </si>
+  <si>
+    <t>EDT8</t>
+  </si>
+  <si>
+    <t>0.713, 0</t>
+  </si>
+  <si>
+    <t>EDT9</t>
+  </si>
+  <si>
+    <t>0.728, 0</t>
+  </si>
+  <si>
+    <t>EDT10</t>
+  </si>
+  <si>
+    <t>0.746, 0</t>
+  </si>
+  <si>
+    <t>EDT11</t>
+  </si>
+  <si>
+    <t>0.776, 0</t>
+  </si>
+  <si>
+    <t>EDT12</t>
+  </si>
+  <si>
+    <t>0.808, 0</t>
+  </si>
+  <si>
+    <t>EDT13</t>
+  </si>
+  <si>
+    <t>0.835, 0</t>
+  </si>
+  <si>
+    <t>EDT14</t>
+  </si>
+  <si>
+    <t>0.86, 0</t>
+  </si>
+  <si>
+    <t>EDT15</t>
+  </si>
+  <si>
+    <t>0.879, 0</t>
+  </si>
+  <si>
+    <t>EDT16</t>
+  </si>
+  <si>
+    <t>0.922, 0</t>
+  </si>
+  <si>
+    <t>EDT17</t>
+  </si>
+  <si>
+    <t>0.954, 0</t>
+  </si>
+  <si>
+    <t>EDT18</t>
+  </si>
+  <si>
+    <t>0.996, 0</t>
+  </si>
+  <si>
+    <t>EDT19</t>
+  </si>
+  <si>
+    <t>1, 0</t>
+  </si>
+  <si>
+    <t>EDT20</t>
+  </si>
+  <si>
+    <t>0.986, 0</t>
+  </si>
+  <si>
+    <t>EDT21</t>
+  </si>
+  <si>
+    <t>0.949, 0</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>EDT22</t>
+  </si>
+  <si>
+    <t>0.901, 0</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>EDT23</t>
+  </si>
+  <si>
+    <t>0.823, 0</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>EDT24</t>
+  </si>
+  <si>
+    <t>0.737, 0</t>
+  </si>
+  <si>
+    <t>UCT7</t>
+  </si>
+  <si>
+    <t>UCT8</t>
+  </si>
+  <si>
+    <t>UCT9</t>
+  </si>
+  <si>
+    <t>UCT10</t>
+  </si>
+  <si>
+    <t>UCT11</t>
+  </si>
+  <si>
+    <t>UCT12</t>
+  </si>
+  <si>
+    <t>UCT13</t>
+  </si>
+  <si>
+    <t>UCT14</t>
+  </si>
+  <si>
+    <t>UCT15</t>
+  </si>
+  <si>
+    <t>UCT16</t>
+  </si>
+  <si>
+    <t>UCT17</t>
+  </si>
+  <si>
+    <t>UCT18</t>
+  </si>
+  <si>
+    <t>UCT19</t>
+  </si>
+  <si>
+    <t>UCT20</t>
+  </si>
+  <si>
+    <t>UCT21</t>
+  </si>
+  <si>
+    <t>UCT22</t>
+  </si>
+  <si>
+    <t>UCT23</t>
+  </si>
+  <si>
+    <t>UCT24</t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>Dcost_1</t>
+  </si>
+  <si>
+    <t>Dcost_2</t>
+  </si>
+  <si>
+    <t>Dcost_3</t>
+  </si>
+  <si>
+    <t>Dcost_4</t>
+  </si>
+  <si>
+    <t>Dcost_5</t>
+  </si>
+  <si>
+    <t>Dcost_6</t>
+  </si>
+  <si>
+    <t>Dcost_7</t>
+  </si>
+  <si>
+    <t>Dcost_8</t>
+  </si>
+  <si>
+    <t>Dcost_9</t>
+  </si>
+  <si>
+    <t>Dcost_10</t>
+  </si>
+  <si>
+    <t>Dcost_11</t>
+  </si>
+  <si>
+    <t>csr</t>
+  </si>
+  <si>
+    <t>SRC_1</t>
+  </si>
+  <si>
+    <t>SRC_2</t>
+  </si>
+  <si>
+    <t>SRC_3</t>
+  </si>
+  <si>
+    <t>SRC_4</t>
+  </si>
+  <si>
+    <t>SRC_5</t>
+  </si>
+  <si>
+    <t>cnsr</t>
+  </si>
+  <si>
+    <t>NSRC_1</t>
+  </si>
+  <si>
+    <t>NSRC_2</t>
+  </si>
+  <si>
+    <t>NSRC_3</t>
+  </si>
+  <si>
+    <t>NSRC_4</t>
+  </si>
+  <si>
+    <t>NSRC_5</t>
   </si>
 </sst>
 </file>
@@ -929,13 +1178,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -994,6 +1236,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1003,7 +1253,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1052,45 +1302,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1431,10 +1699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C580AE-BCDB-6447-87F2-91D4F169EC59}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1471,8 +1739,30 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C4" t="s">
+        <v>288</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1530,7 +1820,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -1538,10 +1828,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD46B62-3884-454B-83D5-13A7DC1C4BB6}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection sqref="A1:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1553,95 +1843,361 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" s="12"/>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>256</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>257</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>258</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>259</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>260</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>261</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>223</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>240</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>324</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>330</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>332</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8DE934-58E4-5047-A795-90496D563932}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="J38" sqref="J38:J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1653,90 +2209,611 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" s="12"/>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>262</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>263</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>264</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>265</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>266</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>267</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>223</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>240</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>324</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>330</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>332</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0AADCB-2F5C-8249-9343-310D36C297B3}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="14">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="14">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="14">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DCD101-2671-4F48-972B-11EA0EF73763}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1760,10 +2837,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>12</v>
@@ -1774,13 +2851,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E2" s="7">
         <v>0.05</v>
@@ -1797,13 +2874,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E3" s="7">
         <v>0.05</v>
@@ -1820,7 +2897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111A03E0-C10C-0D49-95E3-8985E6A9343A}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -1831,104 +2908,104 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>279</v>
+      <c r="D1" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="14">
+      <c r="A2" s="10">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="C2" s="14" t="s">
+      <c r="B2" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="10">
         <v>0</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="14">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="C3" s="14" t="s">
+      <c r="B3" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="10">
         <v>0</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="14">
+      <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="10">
         <v>0</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="14">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="10">
         <v>0</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="14">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="10">
         <v>0</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1937,12 +3014,186 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEFDE885-6D53-A84E-BDCB-CAB019D9A33F}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{495314F4-C3CE-B943-8CDA-C158FD3E3B36}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>367</v>
+      </c>
+      <c r="C4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>368</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>369</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB7A23E-CBBD-454F-8F4F-269AE72EF5B7}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1961,7 +3212,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>12</v>
@@ -1972,16 +3223,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E2" s="7">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>21</v>
@@ -1992,16 +3243,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E3" s="7">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>43</v>
@@ -2012,74 +3263,98 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB7A23E-CBBD-454F-8F4F-269AE72EF5B7}">
-  <dimension ref="A1:F3"/>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC99D2AC-7148-2842-947F-C6D0CB715F06}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="E2" s="7">
-        <v>5</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="E3" s="7">
-        <v>5</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>43</v>
+      <c r="C1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>373</v>
+      </c>
+      <c r="C4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>375</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -2758,7 +4033,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <ignoredErrors>
@@ -2772,7 +4047,7 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView zoomScale="105" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2841,11 +4116,11 @@
       <c r="T1" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="U1" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="V1" s="11" t="s">
-        <v>261</v>
+      <c r="U1" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -2907,10 +4182,10 @@
         <v>1</v>
       </c>
       <c r="U2" s="1">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="V2" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -2972,10 +4247,10 @@
         <v>1</v>
       </c>
       <c r="U3" s="1">
-        <v>45</v>
+        <v>0.5</v>
       </c>
       <c r="V3" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -3037,10 +4312,10 @@
         <v>1</v>
       </c>
       <c r="U4" s="1">
-        <v>40</v>
+        <v>0.5</v>
       </c>
       <c r="V4" s="1">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -3102,14 +4377,14 @@
         <v>1</v>
       </c>
       <c r="U5" s="1">
-        <v>35</v>
+        <v>0.5</v>
       </c>
       <c r="V5" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:S1 A3:D5 A2:D2 F2:S2 F3:S5" numberStoredAsText="1"/>
@@ -3119,10 +4394,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3194,11 +4469,11 @@
       <c r="U1" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="V1" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>261</v>
+      <c r="V1" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -3262,15 +4537,27 @@
       <c r="U2" s="7">
         <v>1</v>
       </c>
-      <c r="V2" s="10">
-        <v>50</v>
-      </c>
-      <c r="W2" s="10">
-        <v>30</v>
-      </c>
+      <c r="V2" s="1">
+        <v>2</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:T1 A2:D2 F2:T2" numberStoredAsText="1"/>
@@ -3707,7 +4994,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:K12" numberStoredAsText="1"/>
@@ -5163,7 +6450,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:X21" numberStoredAsText="1"/>
@@ -5276,7 +6563,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:J3" numberStoredAsText="1"/>
@@ -5337,7 +6624,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:D3" numberStoredAsText="1"/>
@@ -5350,7 +6637,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5530,7 +6817,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:D1 G1:I1 A6:D6 A2:D2 G2:I2 A3:D3 G3:I3 A4:D4 G4:I4 A5:D5 G5:I5 G6:I6" numberStoredAsText="1"/>

</xml_diff>

<commit_message>
Minor fix on cases ieee14 and ieee39
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_uced.xlsx
+++ b/ams/cases/ieee14/ieee14_uced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10402"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9774DCD-763B-2646-B84B-D62DC2047955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72A96D1-5E33-1F4E-83E4-50778F467DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="385">
   <si>
     <t>uid</t>
   </si>
@@ -1797,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2664,7 +2664,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2689,7 +2689,7 @@
         <v>266</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2711,8 +2711,8 @@
       <c r="F2" s="7">
         <v>0.05</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>21</v>
+      <c r="G2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2734,8 +2734,8 @@
       <c r="F3" s="7">
         <v>0.05</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>43</v>
+      <c r="G3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2865,7 +2865,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2887,7 +2887,7 @@
         <v>276</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2906,8 +2906,8 @@
       <c r="E2" s="7">
         <v>0.03</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>21</v>
+      <c r="F2" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2926,8 +2926,8 @@
       <c r="E3" s="7">
         <v>0.03</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>43</v>
+      <c r="F3" s="7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3038,8 +3038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB7A23E-CBBD-454F-8F4F-269AE72EF5B7}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3061,7 +3061,7 @@
         <v>276</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -3080,8 +3080,8 @@
       <c r="E2" s="7">
         <v>0.05</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>21</v>
+      <c r="F2" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -3100,8 +3100,8 @@
       <c r="E3" s="7">
         <v>0.05</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>43</v>
+      <c r="F3" s="7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6680,7 +6680,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:D3"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>